<commit_message>
update plan 20201119 & update result 20201120
</commit_message>
<xml_diff>
--- a/20201119.xlsx
+++ b/20201119.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swan3\Desktop\plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5604C5B-CC0C-429D-AD0F-714A3145F2E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62617964-54AC-4FA1-9BFB-8626FE56FE54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-120" windowWidth="23256" windowHeight="12576" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
   <si>
     <t>일</t>
   </si>
@@ -223,6 +223,10 @@
 </t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
+  <si>
+    <t>술먹음</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -394,7 +398,7 @@
       <charset val="129"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -609,6 +613,30 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -877,7 +905,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -908,24 +936,6 @@
     <xf numFmtId="0" fontId="1" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="1" fillId="32" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -935,20 +945,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="176" fontId="1" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="39" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="40" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="40" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -1482,7 +1522,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E3" sqref="E3:E23"/>
     </sheetView>
   </sheetViews>
@@ -1537,18 +1577,18 @@
       </c>
     </row>
     <row r="3" spans="2:13" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="16" t="s">
+      <c r="D3" s="15"/>
+      <c r="E3" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="23"/>
-      <c r="G3" s="14" t="s">
+      <c r="F3" s="13"/>
+      <c r="G3" s="25" t="s">
         <v>48</v>
       </c>
       <c r="H3" s="8"/>
@@ -1563,12 +1603,12 @@
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B4" s="18"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="14"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="25"/>
       <c r="H4" s="8"/>
       <c r="I4" t="s">
         <v>11</v>
@@ -1578,12 +1618,12 @@
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B5" s="18"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="14"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="25"/>
       <c r="H5" s="8"/>
       <c r="I5" t="s">
         <v>12</v>
@@ -1593,12 +1633,12 @@
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B6" s="18"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="14"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="25"/>
       <c r="H6" s="8"/>
       <c r="I6" t="s">
         <v>10</v>
@@ -1608,12 +1648,12 @@
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B7" s="18"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="14"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="25"/>
       <c r="H7" s="8"/>
       <c r="I7" t="s">
         <v>8</v>
@@ -1627,12 +1667,12 @@
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B8" s="18"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="14"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="25"/>
       <c r="H8" s="8"/>
       <c r="I8" t="s">
         <v>4</v>
@@ -1645,195 +1685,201 @@
       <c r="B9" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="14"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="25"/>
       <c r="H9" s="8"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B10" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="14"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="25"/>
       <c r="H10" s="8"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="14"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="25"/>
       <c r="H11" s="8"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B12" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="14"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="25"/>
       <c r="H12" s="8"/>
     </row>
     <row r="13" spans="2:13" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="14"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="25"/>
       <c r="H13" s="8"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B14" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="14"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="25"/>
       <c r="H14" s="8"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="15"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="26" t="s">
+        <v>50</v>
+      </c>
       <c r="H15" s="8"/>
     </row>
     <row r="16" spans="2:13" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="15"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="27"/>
       <c r="H16" s="8"/>
     </row>
     <row r="17" spans="2:8" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="D17" s="11"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="15"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="27"/>
       <c r="H17" s="8"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B18" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="15"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="27"/>
       <c r="H18" s="8"/>
     </row>
     <row r="19" spans="2:8" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B19" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="11"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="15"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="27"/>
       <c r="H19" s="8"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B20" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="10"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="15"/>
+      <c r="D20" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="10"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="27"/>
       <c r="H20" s="8"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B21" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="15"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="27"/>
       <c r="H21" s="8"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B22" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="15"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="27"/>
       <c r="H22" s="8"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B23" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="13"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="15"/>
+      <c r="D23" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" s="10"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="27"/>
       <c r="H23" s="8"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.4">

</xml_diff>